<commit_message>
Save tested code before refactoring server.js
</commit_message>
<xml_diff>
--- a/backend/uploads/AflPlayers2022.xlsx
+++ b/backend/uploads/AflPlayers2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunil\Projects\footy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB55A03-1313-41A1-A663-9990400B8DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E790F8-CFDF-4880-8F42-214E685C1EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5852" uniqueCount="2472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5853" uniqueCount="2472">
   <si>
     <t>UniqueKey</t>
   </si>
@@ -7819,7 +7819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q777"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
@@ -10723,7 +10723,7 @@
         <v>195</v>
       </c>
       <c r="G60">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H60">
         <v>193</v>
@@ -10748,6 +10748,9 @@
       </c>
       <c r="O60" t="s">
         <v>2462</v>
+      </c>
+      <c r="P60" t="s">
+        <v>2460</v>
       </c>
       <c r="Q60" t="s">
         <v>2462</v>

</xml_diff>